<commit_message>
fixed problem with updating prices
</commit_message>
<xml_diff>
--- a/price_operations/prices_update.xlsx
+++ b/price_operations/prices_update.xlsx
@@ -18,10 +18,10 @@
     <t>price</t>
   </si>
   <si>
-    <t>PigafonePro</t>
+    <t>PigaphoneProXL</t>
   </si>
   <si>
-    <t>Pigomputer Air</t>
+    <t>PigBook Air</t>
   </si>
 </sst>
 </file>
@@ -302,7 +302,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>119999</v>
+        <v>80000</v>
       </c>
     </row>
     <row outlineLevel="0" r="3">
@@ -310,7 +310,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>259999</v>
+        <v>140000</v>
       </c>
     </row>
     <row outlineLevel="0" r="4">

</xml_diff>